<commit_message>
fixed error in overwriting concepts
</commit_message>
<xml_diff>
--- a/t12_segCAMs/outputs/networkIndicators.xlsx
+++ b/t12_segCAMs/outputs/networkIndicators.xlsx
@@ -1015,7 +1015,7 @@
         <v>0.373015873015873</v>
       </c>
       <c r="K2" t="n">
-        <v>0.740385687575861</v>
+        <v>0.7403856875758612</v>
       </c>
       <c r="L2" t="n">
         <v>2.1333333333333333</v>
@@ -1072,16 +1072,16 @@
         <v>-0.3253856942496493</v>
       </c>
       <c r="AD2" t="n">
-        <v>2.5454545454545454</v>
+        <v>8.0</v>
       </c>
       <c r="AE2" t="n">
-        <v>-0.18181818181818182</v>
+        <v>0.0</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.6487658267349983</v>
+        <v>1.0</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.4510582010582011</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="3">
@@ -1116,7 +1116,7 @@
         <v>0.6723484848484849</v>
       </c>
       <c r="K3" t="n">
-        <v>0.7039631414544361</v>
+        <v>0.7039631414544358</v>
       </c>
       <c r="L3" t="n">
         <v>3.5789473684210527</v>
@@ -1173,16 +1173,16 @@
         <v>-0.29971988795518206</v>
       </c>
       <c r="AD3" t="n">
-        <v>2.4615384615384617</v>
+        <v>7.0</v>
       </c>
       <c r="AE3" t="n">
-        <v>-0.46153846153846156</v>
+        <v>-3.0</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.6501952759715706</v>
+        <v>1.0</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.2761904761904762</v>
+        <v>0.0952380952380952</v>
       </c>
     </row>
     <row r="4">
@@ -1217,7 +1217,7 @@
         <v>0.6502525252525253</v>
       </c>
       <c r="K4" t="n">
-        <v>0.6459729144432843</v>
+        <v>0.6459729144432845</v>
       </c>
       <c r="L4" t="n">
         <v>4.181818181818182</v>
@@ -1274,16 +1274,16 @@
         <v>-0.5527777777777781</v>
       </c>
       <c r="AD4" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="AE4" t="n">
-        <v>-0.07692307692307693</v>
+        <v>3.0</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.6658426622412432</v>
+        <v>1.0</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.38888888888888884</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
@@ -1318,7 +1318,7 @@
         <v>0.6742424242424242</v>
       </c>
       <c r="K5" t="n">
-        <v>0.7256314504280087</v>
+        <v>0.7256314504280088</v>
       </c>
       <c r="L5" t="n">
         <v>4.517241379310345</v>
@@ -1375,13 +1375,13 @@
         <v>-0.24414715719063534</v>
       </c>
       <c r="AD5" t="n">
-        <v>1.8461538461538463</v>
+        <v>5.0</v>
       </c>
       <c r="AE5" t="n">
-        <v>-0.8461538461538461</v>
+        <v>0.0</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.6502993020113096</v>
+        <v>1.0</v>
       </c>
       <c r="AG5" t="n">
         <v>0.0</v>
@@ -1476,16 +1476,16 @@
         <v>-0.17293233082706774</v>
       </c>
       <c r="AD6" t="n">
-        <v>2.1666666666666665</v>
+        <v>4.0</v>
       </c>
       <c r="AE6" t="n">
-        <v>-0.6666666666666666</v>
+        <v>-3.0</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.6787931943441321</v>
+        <v>1.0</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.25925925925925924</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
@@ -1520,7 +1520,7 @@
         <v>0.8699494949494949</v>
       </c>
       <c r="K7" t="n">
-        <v>0.7730948816876565</v>
+        <v>0.7730948816876566</v>
       </c>
       <c r="L7" t="n">
         <v>3.391304347826087</v>
@@ -1577,13 +1577,13 @@
         <v>-0.554083885209713</v>
       </c>
       <c r="AD7" t="n">
-        <v>1.8461538461538463</v>
+        <v>8.0</v>
       </c>
       <c r="AE7" t="n">
-        <v>-0.9230769230769231</v>
+        <v>0.0</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.5975908074117794</v>
+        <v>1.0</v>
       </c>
       <c r="AG7" t="n">
         <v>0.0</v>
@@ -1621,7 +1621,7 @@
         <v>0.7950413223140496</v>
       </c>
       <c r="K8" t="n">
-        <v>0.6992949937059291</v>
+        <v>0.6992949937059292</v>
       </c>
       <c r="L8" t="n">
         <v>3.6</v>
@@ -1678,16 +1678,16 @@
         <v>-0.42857142857142855</v>
       </c>
       <c r="AD8" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="AE8" t="n">
-        <v>-0.25</v>
+        <v>0.0</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.6225176889313512</v>
+        <v>1.0</v>
       </c>
       <c r="AG8" t="n">
-        <v>0.38888888888888884</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
@@ -1722,7 +1722,7 @@
         <v>0.40067340067340057</v>
       </c>
       <c r="K9" t="n">
-        <v>0.5001923783242052</v>
+        <v>0.5001923783242048</v>
       </c>
       <c r="L9" t="n">
         <v>3.017543859649123</v>
@@ -1779,16 +1779,16 @@
         <v>-0.12941176470588237</v>
       </c>
       <c r="AD9" t="n">
-        <v>2.4615384615384617</v>
+        <v>4.0</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.07692307692307693</v>
+        <v>0.0</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.7298103016217787</v>
+        <v>1.0</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.15</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
@@ -1823,7 +1823,7 @@
         <v>0.4940828402366864</v>
       </c>
       <c r="K10" t="n">
-        <v>0.6661966366553171</v>
+        <v>0.6661966366553169</v>
       </c>
       <c r="L10" t="n">
         <v>6.016949152542373</v>
@@ -1880,16 +1880,16 @@
         <v>-0.22448979591836785</v>
       </c>
       <c r="AD10" t="n">
-        <v>2.142857142857143</v>
+        <v>3.0</v>
       </c>
       <c r="AE10" t="n">
-        <v>-2.2857142857142856</v>
+        <v>-3.0</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.6928932500574584</v>
+        <v>0.862068965517241</v>
       </c>
       <c r="AG10" t="n">
-        <v>0.16666666666666666</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="11">
@@ -1924,7 +1924,7 @@
         <v>0.4911616161616162</v>
       </c>
       <c r="K11" t="n">
-        <v>0.6687610599583352</v>
+        <v>0.6687610599583357</v>
       </c>
       <c r="L11" t="n">
         <v>6.057142857142857</v>
@@ -1981,16 +1981,16 @@
         <v>0.06306306306306307</v>
       </c>
       <c r="AD11" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="AE11" t="n">
         <v>2.0</v>
       </c>
-      <c r="AE11" t="n">
-        <v>0.46153846153846156</v>
-      </c>
       <c r="AF11" t="n">
-        <v>0.6784584697802</v>
+        <v>1.0</v>
       </c>
       <c r="AG11" t="n">
-        <v>0.09523809523809527</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="12">
@@ -2082,13 +2082,13 @@
         <v>-0.804705882352941</v>
       </c>
       <c r="AD12" t="n">
-        <v>2.0</v>
+        <v>11.0</v>
       </c>
       <c r="AE12" t="n">
-        <v>-1.0769230769230769</v>
+        <v>0.0</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.575090232348297</v>
+        <v>1.0</v>
       </c>
       <c r="AG12" t="n">
         <v>0.0</v>
@@ -2126,7 +2126,7 @@
         <v>0.4683597883597884</v>
       </c>
       <c r="K13" t="n">
-        <v>0.689824832853583</v>
+        <v>0.6898248328535831</v>
       </c>
       <c r="L13" t="n">
         <v>3.7260273972602738</v>
@@ -2183,16 +2183,16 @@
         <v>-0.5165794066317627</v>
       </c>
       <c r="AD13" t="n">
-        <v>2.75</v>
+        <v>3.0</v>
       </c>
       <c r="AE13" t="n">
-        <v>-0.25</v>
+        <v>0.0</v>
       </c>
       <c r="AF13" t="n">
-        <v>0.7398766819611393</v>
+        <v>0.892857142857143</v>
       </c>
       <c r="AG13" t="n">
-        <v>0.09595959595959587</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="14">
@@ -2227,7 +2227,7 @@
         <v>0.5256410256410257</v>
       </c>
       <c r="K14" t="n">
-        <v>0.6445011396907581</v>
+        <v>0.6445011396907582</v>
       </c>
       <c r="L14" t="n">
         <v>4.5</v>
@@ -2284,13 +2284,13 @@
         <v>-0.5440613026819925</v>
       </c>
       <c r="AD14" t="n">
-        <v>1.8571428571428572</v>
+        <v>4.0</v>
       </c>
       <c r="AE14" t="n">
-        <v>-1.7857142857142858</v>
+        <v>-3.0</v>
       </c>
       <c r="AF14" t="n">
-        <v>0.6959949753772947</v>
+        <v>1.0</v>
       </c>
       <c r="AG14" t="n">
         <v>0.0</v>
@@ -2328,7 +2328,7 @@
         <v>1.0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.7759907622602039</v>
+        <v>0.7759907622602042</v>
       </c>
       <c r="L15" t="n">
         <v>1.625</v>
@@ -2385,13 +2385,13 @@
         <v>-1.0</v>
       </c>
       <c r="AD15" t="n">
-        <v>1.8461538461538463</v>
+        <v>12.0</v>
       </c>
       <c r="AE15" t="n">
-        <v>-0.8461538461538461</v>
+        <v>0.0</v>
       </c>
       <c r="AF15" t="n">
-        <v>0.5585284280936459</v>
+        <v>1.0</v>
       </c>
       <c r="AG15" t="n">
         <v>0.0</v>
@@ -2486,13 +2486,13 @@
         <v>-0.8758565094719873</v>
       </c>
       <c r="AD16" t="n">
-        <v>1.8571428571428572</v>
+        <v>12.0</v>
       </c>
       <c r="AE16" t="n">
-        <v>0.2857142857142857</v>
+        <v>3.0</v>
       </c>
       <c r="AF16" t="n">
-        <v>0.5639499389499386</v>
+        <v>1.0</v>
       </c>
       <c r="AG16" t="n">
         <v>0.0</v>
@@ -2530,7 +2530,7 @@
         <v>0.8005050505050505</v>
       </c>
       <c r="K17" t="n">
-        <v>0.7094200825169517</v>
+        <v>0.7094200825169515</v>
       </c>
       <c r="L17" t="n">
         <v>3.425925925925926</v>
@@ -2587,16 +2587,16 @@
         <v>-0.46527777777777773</v>
       </c>
       <c r="AD17" t="n">
-        <v>2.923076923076923</v>
+        <v>11.0</v>
       </c>
       <c r="AE17" t="n">
-        <v>-1.0769230769230769</v>
+        <v>-3.0</v>
       </c>
       <c r="AF17" t="n">
-        <v>0.5990209971188233</v>
+        <v>1.0</v>
       </c>
       <c r="AG17" t="n">
-        <v>0.7539944903581267</v>
+        <v>0.127272727272727</v>
       </c>
     </row>
     <row r="18">
@@ -2631,7 +2631,7 @@
         <v>0.5943458251150558</v>
       </c>
       <c r="K18" t="n">
-        <v>0.6384209554272583</v>
+        <v>0.6384209554272582</v>
       </c>
       <c r="L18" t="n">
         <v>5.568181818181818</v>
@@ -2688,13 +2688,13 @@
         <v>-0.28859060402684567</v>
       </c>
       <c r="AD18" t="n">
-        <v>2.2857142857142856</v>
+        <v>5.0</v>
       </c>
       <c r="AE18" t="n">
-        <v>-1.2857142857142858</v>
+        <v>-3.0</v>
       </c>
       <c r="AF18" t="n">
-        <v>0.6605215860034092</v>
+        <v>1.0</v>
       </c>
       <c r="AG18" t="n">
         <v>0.0</v>
@@ -2732,7 +2732,7 @@
         <v>0.4659090909090909</v>
       </c>
       <c r="K19" t="n">
-        <v>0.6800727431914514</v>
+        <v>0.6800727431914516</v>
       </c>
       <c r="L19" t="n">
         <v>1.641025641025641</v>
@@ -2789,16 +2789,16 @@
         <v>-0.13586956521739185</v>
       </c>
       <c r="AD19" t="n">
-        <v>2.923076923076923</v>
+        <v>5.0</v>
       </c>
       <c r="AE19" t="n">
-        <v>-0.6923076923076923</v>
+        <v>0.0</v>
       </c>
       <c r="AF19" t="n">
-        <v>0.709651248540978</v>
+        <v>1.0</v>
       </c>
       <c r="AG19" t="n">
-        <v>0.4611111111111111</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="20">
@@ -2833,7 +2833,7 @@
         <v>0.18543956043956045</v>
       </c>
       <c r="K20" t="n">
-        <v>0.5836291076644483</v>
+        <v>0.583629107664448</v>
       </c>
       <c r="L20" t="n">
         <v>5.4520547945205475</v>
@@ -2890,16 +2890,16 @@
         <v>-0.02678571428571349</v>
       </c>
       <c r="AD20" t="n">
-        <v>3.066666666666667</v>
+        <v>2.0</v>
       </c>
       <c r="AE20" t="n">
-        <v>-1.0</v>
+        <v>-2.0</v>
       </c>
       <c r="AF20" t="n">
-        <v>0.8223141042109626</v>
+        <v>0.882352941176471</v>
       </c>
       <c r="AG20" t="n">
-        <v>0.32619047619047614</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21">
@@ -2991,16 +2991,16 @@
         <v>-0.06578947368421083</v>
       </c>
       <c r="AD21" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="AE21" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AF21" t="n">
-        <v>0.6369399821769232</v>
+        <v>1.0</v>
       </c>
       <c r="AG21" t="n">
-        <v>0.09583333333333324</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="22">
@@ -3035,7 +3035,7 @@
         <v>0.8648915187376726</v>
       </c>
       <c r="K22" t="n">
-        <v>0.780259303852818</v>
+        <v>0.7802593038528182</v>
       </c>
       <c r="L22" t="n">
         <v>1.7222222222222223</v>
@@ -3092,13 +3092,13 @@
         <v>-0.464546056991385</v>
       </c>
       <c r="AD22" t="n">
-        <v>1.8571428571428572</v>
+        <v>8.0</v>
       </c>
       <c r="AE22" t="n">
-        <v>-0.35714285714285715</v>
+        <v>0.0</v>
       </c>
       <c r="AF22" t="n">
-        <v>0.5941605387094109</v>
+        <v>1.0</v>
       </c>
       <c r="AG22" t="n">
         <v>0.0</v>
@@ -3136,7 +3136,7 @@
         <v>0.5482731554160125</v>
       </c>
       <c r="K23" t="n">
-        <v>0.6305888847153067</v>
+        <v>0.6305888847153068</v>
       </c>
       <c r="L23" t="n">
         <v>3.0833333333333335</v>
@@ -3193,16 +3193,16 @@
         <v>-0.23021582733813</v>
       </c>
       <c r="AD23" t="n">
-        <v>2.533333333333333</v>
+        <v>5.0</v>
       </c>
       <c r="AE23" t="n">
-        <v>-1.2</v>
+        <v>-2.0</v>
       </c>
       <c r="AF23" t="n">
-        <v>0.7007642043061327</v>
+        <v>1.0</v>
       </c>
       <c r="AG23" t="n">
-        <v>0.36666666666666653</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="24">
@@ -3237,7 +3237,7 @@
         <v>0.7389473684210527</v>
       </c>
       <c r="K24" t="n">
-        <v>0.7562500316434445</v>
+        <v>0.756250031643444</v>
       </c>
       <c r="L24" t="n">
         <v>2.0943396226415096</v>
@@ -3294,13 +3294,13 @@
         <v>-0.37978339350180496</v>
       </c>
       <c r="AD24" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="AE24" t="n">
-        <v>-0.09523809523809523</v>
+        <v>0.0</v>
       </c>
       <c r="AF24" t="n">
-        <v>0.6128908037272442</v>
+        <v>1.0</v>
       </c>
       <c r="AG24" t="n">
         <v>0.0</v>
@@ -3338,7 +3338,7 @@
         <v>0.44938973063973064</v>
       </c>
       <c r="K25" t="n">
-        <v>0.560429292371735</v>
+        <v>0.5604292923717346</v>
       </c>
       <c r="L25" t="n">
         <v>2.1327433628318584</v>
@@ -3395,16 +3395,16 @@
         <v>-0.3360488798370672</v>
       </c>
       <c r="AD25" t="n">
-        <v>4.923076923076923</v>
+        <v>12.0</v>
       </c>
       <c r="AE25" t="n">
-        <v>-0.23076923076923078</v>
+        <v>-3.0</v>
       </c>
       <c r="AF25" t="n">
-        <v>0.6435094317447259</v>
+        <v>1.0</v>
       </c>
       <c r="AG25" t="n">
-        <v>0.7266067266067268</v>
+        <v>0.303030303030303</v>
       </c>
     </row>
     <row r="26">
@@ -3439,7 +3439,7 @@
         <v>0.7901041666666667</v>
       </c>
       <c r="K26" t="n">
-        <v>0.78484168093447</v>
+        <v>0.7848416809344698</v>
       </c>
       <c r="L26" t="n">
         <v>3.7674418604651163</v>
@@ -3496,16 +3496,16 @@
         <v>-0.193702290076336</v>
       </c>
       <c r="AD26" t="n">
-        <v>2.1176470588235294</v>
+        <v>8.0</v>
       </c>
       <c r="AE26" t="n">
-        <v>-0.35294117647058826</v>
+        <v>-3.0</v>
       </c>
       <c r="AF26" t="n">
-        <v>0.602849722852135</v>
+        <v>1.0</v>
       </c>
       <c r="AG26" t="n">
-        <v>0.23015873015873003</v>
+        <v>0.0714285714285714</v>
       </c>
     </row>
     <row r="27">
@@ -3540,7 +3540,7 @@
         <v>0.9818181818181818</v>
       </c>
       <c r="K27" t="n">
-        <v>0.7561930600795044</v>
+        <v>0.7561930600795043</v>
       </c>
       <c r="L27" t="n">
         <v>2.6666666666666665</v>
@@ -3597,16 +3597,16 @@
         <v>-0.888</v>
       </c>
       <c r="AD27" t="n">
-        <v>2.0</v>
+        <v>11.0</v>
       </c>
       <c r="AE27" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.0</v>
       </c>
       <c r="AF27" t="n">
-        <v>0.567857142857143</v>
+        <v>1.0</v>
       </c>
       <c r="AG27" t="n">
-        <v>0.6727272727272727</v>
+        <v>0.0181818181818182</v>
       </c>
     </row>
     <row r="28">
@@ -3641,7 +3641,7 @@
         <v>0.29945286195286186</v>
       </c>
       <c r="K28" t="n">
-        <v>0.6165075123235558</v>
+        <v>0.6165075123235563</v>
       </c>
       <c r="L28" t="n">
         <v>4.67741935483871</v>
@@ -3698,16 +3698,16 @@
         <v>-0.31933842239185756</v>
       </c>
       <c r="AD28" t="n">
-        <v>2.6153846153846154</v>
+        <v>5.0</v>
       </c>
       <c r="AE28" t="n">
-        <v>-2.5384615384615383</v>
+        <v>-3.0</v>
       </c>
       <c r="AF28" t="n">
-        <v>0.7458684432009495</v>
+        <v>1.0</v>
       </c>
       <c r="AG28" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="29">
@@ -3742,7 +3742,7 @@
         <v>0.5276134122287969</v>
       </c>
       <c r="K29" t="n">
-        <v>0.6452743060553274</v>
+        <v>0.6452743060553275</v>
       </c>
       <c r="L29" t="n">
         <v>6.611111111111111</v>
@@ -3799,16 +3799,16 @@
         <v>-0.40816326530612274</v>
       </c>
       <c r="AD29" t="n">
-        <v>2.142857142857143</v>
+        <v>4.0</v>
       </c>
       <c r="AE29" t="n">
-        <v>-1.0</v>
+        <v>-3.0</v>
       </c>
       <c r="AF29" t="n">
-        <v>0.6939008555307139</v>
+        <v>1.0</v>
       </c>
       <c r="AG29" t="n">
-        <v>0.16666666666666666</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="30">
@@ -3900,16 +3900,16 @@
         <v>-0.3480801335559264</v>
       </c>
       <c r="AD30" t="n">
-        <v>2.2666666666666666</v>
+        <v>7.0</v>
       </c>
       <c r="AE30" t="n">
-        <v>-1.0666666666666667</v>
+        <v>0.0</v>
       </c>
       <c r="AF30" t="n">
-        <v>0.6507524701168798</v>
+        <v>1.0</v>
       </c>
       <c r="AG30" t="n">
-        <v>0.1255411255411255</v>
+        <v>0.0476190476190476</v>
       </c>
     </row>
     <row r="31">
@@ -4001,16 +4001,16 @@
         <v>-0.2480620155038759</v>
       </c>
       <c r="AD31" t="n">
-        <v>3.111111111111111</v>
+        <v>7.0</v>
       </c>
       <c r="AE31" t="n">
-        <v>-1.3888888888888888</v>
+        <v>-3.0</v>
       </c>
       <c r="AF31" t="n">
-        <v>0.6957114498065575</v>
+        <v>1.0</v>
       </c>
       <c r="AG31" t="n">
-        <v>0.261344537815126</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="32">
@@ -4045,7 +4045,7 @@
         <v>0.648989898989899</v>
       </c>
       <c r="K32" t="n">
-        <v>0.6614982610536001</v>
+        <v>0.6614982610536</v>
       </c>
       <c r="L32" t="n">
         <v>3.28</v>
@@ -4102,16 +4102,16 @@
         <v>-0.8752997601918464</v>
       </c>
       <c r="AD32" t="n">
-        <v>3.076923076923077</v>
+        <v>9.0</v>
       </c>
       <c r="AE32" t="n">
-        <v>-0.23076923076923078</v>
+        <v>-2.0</v>
       </c>
       <c r="AF32" t="n">
-        <v>0.5945272119185161</v>
+        <v>0.8</v>
       </c>
       <c r="AG32" t="n">
-        <v>0.8343434343434343</v>
+        <v>0.222222222222222</v>
       </c>
     </row>
     <row r="33">
@@ -4146,7 +4146,7 @@
         <v>0.3869165023011177</v>
       </c>
       <c r="K33" t="n">
-        <v>0.5535908241110464</v>
+        <v>0.5535908241110465</v>
       </c>
       <c r="L33" t="n">
         <v>5.504504504504505</v>
@@ -4203,16 +4203,16 @@
         <v>-0.2481997119539121</v>
       </c>
       <c r="AD33" t="n">
-        <v>3.7142857142857144</v>
+        <v>8.0</v>
       </c>
       <c r="AE33" t="n">
-        <v>-1.3571428571428572</v>
+        <v>-3.0</v>
       </c>
       <c r="AF33" t="n">
-        <v>0.7241026817831273</v>
+        <v>1.0</v>
       </c>
       <c r="AG33" t="n">
-        <v>0.26717687074829916</v>
+        <v>0.107142857142857</v>
       </c>
     </row>
     <row r="34">
@@ -4304,13 +4304,13 @@
         <v>-0.2099056603773584</v>
       </c>
       <c r="AD34" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="AE34" t="n">
-        <v>-1.1666666666666667</v>
+        <v>-2.0</v>
       </c>
       <c r="AF34" t="n">
-        <v>0.6266092996457882</v>
+        <v>1.0</v>
       </c>
       <c r="AG34" t="n">
         <v>0.0</v>
@@ -4348,7 +4348,7 @@
         <v>0.5355371900826447</v>
       </c>
       <c r="K35" t="n">
-        <v>0.679461501597685</v>
+        <v>0.6794615015976848</v>
       </c>
       <c r="L35" t="n">
         <v>3.55</v>
@@ -4405,13 +4405,13 @@
         <v>-0.07317073170731705</v>
       </c>
       <c r="AD35" t="n">
-        <v>1.8333333333333333</v>
+        <v>4.0</v>
       </c>
       <c r="AE35" t="n">
-        <v>-2.25</v>
+        <v>0.0</v>
       </c>
       <c r="AF35" t="n">
-        <v>0.7010488555325511</v>
+        <v>1.0</v>
       </c>
       <c r="AG35" t="n">
         <v>0.0</v>
@@ -4449,7 +4449,7 @@
         <v>0.3194662480376766</v>
       </c>
       <c r="K36" t="n">
-        <v>0.6561121091631203</v>
+        <v>0.6561121091631205</v>
       </c>
       <c r="L36" t="n">
         <v>4.222222222222222</v>
@@ -4506,16 +4506,16 @@
         <v>-0.43116883116883137</v>
       </c>
       <c r="AD36" t="n">
-        <v>2.533333333333333</v>
+        <v>5.0</v>
       </c>
       <c r="AE36" t="n">
-        <v>-1.1333333333333333</v>
+        <v>-3.0</v>
       </c>
       <c r="AF36" t="n">
-        <v>0.6847745550427498</v>
+        <v>1.0</v>
       </c>
       <c r="AG36" t="n">
-        <v>0.40952380952380957</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="37">
@@ -4550,7 +4550,7 @@
         <v>0.6734375</v>
       </c>
       <c r="K37" t="n">
-        <v>0.7192975424790956</v>
+        <v>0.7192975424790959</v>
       </c>
       <c r="L37" t="n">
         <v>3.8461538461538463</v>
@@ -4607,16 +4607,16 @@
         <v>-0.12888888888888894</v>
       </c>
       <c r="AD37" t="n">
-        <v>2.823529411764706</v>
+        <v>8.0</v>
       </c>
       <c r="AE37" t="n">
-        <v>-1.6470588235294117</v>
+        <v>-3.0</v>
       </c>
       <c r="AF37" t="n">
-        <v>0.6256927214235076</v>
+        <v>1.0</v>
       </c>
       <c r="AG37" t="n">
-        <v>0.6526785714285713</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="38">
@@ -4651,7 +4651,7 @@
         <v>0.7159090909090909</v>
       </c>
       <c r="K38" t="n">
-        <v>0.6948826958819586</v>
+        <v>0.6948826958819585</v>
       </c>
       <c r="L38" t="n">
         <v>6.519230769230769</v>
@@ -4708,13 +4708,13 @@
         <v>-0.8387096774193549</v>
       </c>
       <c r="AD38" t="n">
-        <v>1.8461538461538463</v>
+        <v>7.0</v>
       </c>
       <c r="AE38" t="n">
-        <v>-2.230769230769231</v>
+        <v>0.0</v>
       </c>
       <c r="AF38" t="n">
-        <v>0.6552566207738619</v>
+        <v>1.0</v>
       </c>
       <c r="AG38" t="n">
         <v>0.0</v>
@@ -4752,7 +4752,7 @@
         <v>0.7746539792387545</v>
       </c>
       <c r="K39" t="n">
-        <v>0.7448042470895524</v>
+        <v>0.7448042470895522</v>
       </c>
       <c r="L39" t="n">
         <v>4.2272727272727275</v>
@@ -4809,16 +4809,16 @@
         <v>-0.3277525022747954</v>
       </c>
       <c r="AD39" t="n">
-        <v>2.6666666666666665</v>
+        <v>10.0</v>
       </c>
       <c r="AE39" t="n">
-        <v>-0.6666666666666666</v>
+        <v>-3.0</v>
       </c>
       <c r="AF39" t="n">
-        <v>0.6110314654283273</v>
+        <v>1.0</v>
       </c>
       <c r="AG39" t="n">
-        <v>0.2341880341880342</v>
+        <v>0.0444444444444444</v>
       </c>
     </row>
     <row r="40">
@@ -4853,7 +4853,7 @@
         <v>0.8446969696969697</v>
       </c>
       <c r="K40" t="n">
-        <v>0.7067166389319381</v>
+        <v>0.7067166389319384</v>
       </c>
       <c r="L40" t="n">
         <v>1.8387096774193548</v>
@@ -4910,16 +4910,16 @@
         <v>-0.561933955691793</v>
       </c>
       <c r="AD40" t="n">
-        <v>2.923076923076923</v>
+        <v>12.0</v>
       </c>
       <c r="AE40" t="n">
-        <v>-2.3846153846153846</v>
+        <v>0.0</v>
       </c>
       <c r="AF40" t="n">
-        <v>0.5851366025279067</v>
+        <v>1.0</v>
       </c>
       <c r="AG40" t="n">
-        <v>0.7606060606060607</v>
+        <v>0.106060606060606</v>
       </c>
     </row>
     <row r="41">
@@ -4954,7 +4954,7 @@
         <v>0.7919132149901381</v>
       </c>
       <c r="K41" t="n">
-        <v>0.747294727145469</v>
+        <v>0.7472947271454687</v>
       </c>
       <c r="L41" t="n">
         <v>4.131578947368421</v>
@@ -5011,13 +5011,13 @@
         <v>-0.26729559748427667</v>
       </c>
       <c r="AD41" t="n">
-        <v>1.8571428571428572</v>
+        <v>6.0</v>
       </c>
       <c r="AE41" t="n">
-        <v>0.5</v>
+        <v>0.0</v>
       </c>
       <c r="AF41" t="n">
-        <v>0.6103290506485994</v>
+        <v>1.0</v>
       </c>
       <c r="AG41" t="n">
         <v>0.0</v>
@@ -5055,7 +5055,7 @@
         <v>0.6300505050505051</v>
       </c>
       <c r="K42" t="n">
-        <v>0.6814509521019753</v>
+        <v>0.6814509521019756</v>
       </c>
       <c r="L42" t="n">
         <v>1.4838709677419355</v>
@@ -5112,16 +5112,16 @@
         <v>-0.19847743338771093</v>
       </c>
       <c r="AD42" t="n">
-        <v>2.923076923076923</v>
+        <v>8.0</v>
       </c>
       <c r="AE42" t="n">
-        <v>-2.769230769230769</v>
+        <v>0.0</v>
       </c>
       <c r="AF42" t="n">
-        <v>0.6541393906830052</v>
+        <v>1.0</v>
       </c>
       <c r="AG42" t="n">
-        <v>0.47321428571428575</v>
+        <v>0.178571428571429</v>
       </c>
     </row>
     <row r="43">
@@ -5213,16 +5213,16 @@
         <v>-0.35285505124451</v>
       </c>
       <c r="AD43" t="n">
-        <v>3.6666666666666665</v>
+        <v>7.0</v>
       </c>
       <c r="AE43" t="n">
-        <v>-1.3333333333333333</v>
+        <v>-3.0</v>
       </c>
       <c r="AF43" t="n">
-        <v>0.7593142584334197</v>
+        <v>1.0</v>
       </c>
       <c r="AG43" t="n">
-        <v>0.4515873015873016</v>
+        <v>0.285714285714286</v>
       </c>
     </row>
     <row r="44">
@@ -5257,7 +5257,7 @@
         <v>0.3963893249607535</v>
       </c>
       <c r="K44" t="n">
-        <v>0.5528351157564725</v>
+        <v>0.5528351157564726</v>
       </c>
       <c r="L44" t="n">
         <v>6.206185567010309</v>
@@ -5314,16 +5314,16 @@
         <v>-0.12340425531914963</v>
       </c>
       <c r="AD44" t="n">
-        <v>3.2</v>
+        <v>5.0</v>
       </c>
       <c r="AE44" t="n">
-        <v>-0.8666666666666667</v>
+        <v>0.0</v>
       </c>
       <c r="AF44" t="n">
-        <v>0.7149008725268416</v>
+        <v>1.0</v>
       </c>
       <c r="AG44" t="n">
-        <v>0.2733333333333333</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="45">
@@ -5358,7 +5358,7 @@
         <v>0.31786948853615515</v>
       </c>
       <c r="K45" t="n">
-        <v>0.6109976549649965</v>
+        <v>0.6109976549649964</v>
       </c>
       <c r="L45" t="n">
         <v>2.888</v>
@@ -5415,16 +5415,16 @@
         <v>-0.38461538461538464</v>
       </c>
       <c r="AD45" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="AE45" t="n">
-        <v>-0.6875</v>
+        <v>-3.0</v>
       </c>
       <c r="AF45" t="n">
-        <v>0.7074221693761219</v>
+        <v>0.689655172413793</v>
       </c>
       <c r="AG45" t="n">
-        <v>0.35619047619047617</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="46">
@@ -5459,7 +5459,7 @@
         <v>0.8598484848484849</v>
       </c>
       <c r="K46" t="n">
-        <v>0.7117226763030792</v>
+        <v>0.7117226763030794</v>
       </c>
       <c r="L46" t="n">
         <v>4.1</v>
@@ -5516,16 +5516,16 @@
         <v>-0.6380697050938341</v>
       </c>
       <c r="AD46" t="n">
-        <v>2.769230769230769</v>
+        <v>12.0</v>
       </c>
       <c r="AE46" t="n">
-        <v>-1.3846153846153846</v>
+        <v>0.0</v>
       </c>
       <c r="AF46" t="n">
-        <v>0.581488077140251</v>
+        <v>1.0</v>
       </c>
       <c r="AG46" t="n">
-        <v>0.6988636363636365</v>
+        <v>0.0909090909090909</v>
       </c>
     </row>
     <row r="47">
@@ -5560,7 +5560,7 @@
         <v>0.9002525252525253</v>
       </c>
       <c r="K47" t="n">
-        <v>0.7584884506513884</v>
+        <v>0.758488450651388</v>
       </c>
       <c r="L47" t="n">
         <v>2.7142857142857144</v>
@@ -5617,16 +5617,16 @@
         <v>-0.6614210777300907</v>
       </c>
       <c r="AD47" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="AE47" t="n">
-        <v>-0.23076923076923078</v>
+        <v>0.0</v>
       </c>
       <c r="AF47" t="n">
-        <v>0.5931808576039346</v>
+        <v>1.0</v>
       </c>
       <c r="AG47" t="n">
-        <v>0.4666666666666666</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="48">
@@ -5718,13 +5718,13 @@
         <v>-1.0</v>
       </c>
       <c r="AD48" t="n">
-        <v>1.8461538461538463</v>
+        <v>12.0</v>
       </c>
       <c r="AE48" t="n">
-        <v>-0.15384615384615385</v>
+        <v>-1.0</v>
       </c>
       <c r="AF48" t="n">
-        <v>0.5585284280936459</v>
+        <v>1.0</v>
       </c>
       <c r="AG48" t="n">
         <v>0.0</v>
@@ -5762,7 +5762,7 @@
         <v>0.6429752066115703</v>
       </c>
       <c r="K49" t="n">
-        <v>0.6001663826186264</v>
+        <v>0.6001663826186265</v>
       </c>
       <c r="L49" t="n">
         <v>3.462686567164179</v>
@@ -5819,16 +5819,16 @@
         <v>-0.37931034482758624</v>
       </c>
       <c r="AD49" t="n">
-        <v>3.8333333333333335</v>
+        <v>10.0</v>
       </c>
       <c r="AE49" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AF49" t="n">
-        <v>0.6488269470467615</v>
+        <v>1.0</v>
       </c>
       <c r="AG49" t="n">
-        <v>0.6414141414141414</v>
+        <v>0.222222222222222</v>
       </c>
     </row>
     <row r="50">
@@ -5863,7 +5863,7 @@
         <v>0.5795454545454546</v>
       </c>
       <c r="K50" t="n">
-        <v>0.5876751203535702</v>
+        <v>0.5876751203535705</v>
       </c>
       <c r="L50" t="n">
         <v>1.52</v>
@@ -5920,13 +5920,13 @@
         <v>-0.9882491186839014</v>
       </c>
       <c r="AD50" t="n">
-        <v>1.8461538461538463</v>
+        <v>2.0</v>
       </c>
       <c r="AE50" t="n">
         <v>0.0</v>
       </c>
       <c r="AF50" t="n">
-        <v>0.7218178241196146</v>
+        <v>1.0</v>
       </c>
       <c r="AG50" t="n">
         <v>0.0</v>
@@ -5964,7 +5964,7 @@
         <v>0.8793388429752066</v>
       </c>
       <c r="K51" t="n">
-        <v>0.7649371473690574</v>
+        <v>0.7649371473690575</v>
       </c>
       <c r="L51" t="n">
         <v>1.6666666666666667</v>
@@ -6021,13 +6021,13 @@
         <v>-0.6559139784946237</v>
       </c>
       <c r="AD51" t="n">
-        <v>1.8333333333333333</v>
+        <v>8.0</v>
       </c>
       <c r="AE51" t="n">
-        <v>-0.08333333333333333</v>
+        <v>0.0</v>
       </c>
       <c r="AF51" t="n">
-        <v>0.6005997474747473</v>
+        <v>1.0</v>
       </c>
       <c r="AG51" t="n">
         <v>0.0</v>
@@ -6065,7 +6065,7 @@
         <v>0.8181818181818182</v>
       </c>
       <c r="K52" t="n">
-        <v>0.6991548881373775</v>
+        <v>0.6991548881373778</v>
       </c>
       <c r="L52" t="n">
         <v>3.4375</v>
@@ -6122,16 +6122,16 @@
         <v>-0.6112621359223303</v>
       </c>
       <c r="AD52" t="n">
-        <v>2.769230769230769</v>
+        <v>11.0</v>
       </c>
       <c r="AE52" t="n">
-        <v>-0.6153846153846154</v>
+        <v>0.0</v>
       </c>
       <c r="AF52" t="n">
-        <v>0.6016432868796162</v>
+        <v>1.0</v>
       </c>
       <c r="AG52" t="n">
-        <v>0.7582491582491583</v>
+        <v>0.0909090909090909</v>
       </c>
     </row>
     <row r="53">
@@ -6223,13 +6223,13 @@
         <v>-1.0</v>
       </c>
       <c r="AD53" t="n">
-        <v>1.8461538461538463</v>
+        <v>12.0</v>
       </c>
       <c r="AE53" t="n">
-        <v>0.38461538461538464</v>
+        <v>0.0</v>
       </c>
       <c r="AF53" t="n">
-        <v>0.5585284280936459</v>
+        <v>1.0</v>
       </c>
       <c r="AG53" t="n">
         <v>0.0</v>
@@ -6267,7 +6267,7 @@
         <v>0.827020202020202</v>
       </c>
       <c r="K54" t="n">
-        <v>0.7608344969958328</v>
+        <v>0.7608344969958327</v>
       </c>
       <c r="L54" t="n">
         <v>3.1621621621621623</v>
@@ -6324,13 +6324,13 @@
         <v>-0.479638009049774</v>
       </c>
       <c r="AD54" t="n">
-        <v>1.8461538461538463</v>
+        <v>7.0</v>
       </c>
       <c r="AE54" t="n">
-        <v>0.23076923076923078</v>
+        <v>0.0</v>
       </c>
       <c r="AF54" t="n">
-        <v>0.6078000654923732</v>
+        <v>1.0</v>
       </c>
       <c r="AG54" t="n">
         <v>0.0</v>
@@ -6368,7 +6368,7 @@
         <v>0.2632996632996633</v>
       </c>
       <c r="K55" t="n">
-        <v>0.5579632877250357</v>
+        <v>0.5579632877250358</v>
       </c>
       <c r="L55" t="n">
         <v>4.096774193548387</v>
@@ -6425,16 +6425,16 @@
         <v>-0.25148514851485176</v>
       </c>
       <c r="AD55" t="n">
-        <v>4.3076923076923075</v>
+        <v>6.0</v>
       </c>
       <c r="AE55" t="n">
-        <v>1.2307692307692308</v>
+        <v>0.0</v>
       </c>
       <c r="AF55" t="n">
-        <v>0.7186196555893791</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="AG55" t="n">
-        <v>0.5611111111111111</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="56">
@@ -6469,7 +6469,7 @@
         <v>1.0</v>
       </c>
       <c r="K56" t="n">
-        <v>0.7683375209644598</v>
+        <v>0.7683375209644601</v>
       </c>
       <c r="L56" t="n">
         <v>2.1379310344827585</v>
@@ -6526,13 +6526,13 @@
         <v>-1.0</v>
       </c>
       <c r="AD56" t="n">
-        <v>1.8333333333333333</v>
+        <v>11.0</v>
       </c>
       <c r="AE56" t="n">
-        <v>-0.4166666666666667</v>
+        <v>0.0</v>
       </c>
       <c r="AF56" t="n">
-        <v>0.5634920634920636</v>
+        <v>1.0</v>
       </c>
       <c r="AG56" t="n">
         <v>0.0</v>
@@ -6570,7 +6570,7 @@
         <v>0.7001972386587771</v>
       </c>
       <c r="K57" t="n">
-        <v>0.7214725650655627</v>
+        <v>0.721472565065563</v>
       </c>
       <c r="L57" t="n">
         <v>4.585365853658536</v>
@@ -6627,13 +6627,13 @@
         <v>-0.48477157360406076</v>
       </c>
       <c r="AD57" t="n">
-        <v>1.8571428571428572</v>
+        <v>5.0</v>
       </c>
       <c r="AE57" t="n">
-        <v>-0.42857142857142855</v>
+        <v>0.0</v>
       </c>
       <c r="AF57" t="n">
-        <v>0.6396799641187764</v>
+        <v>1.0</v>
       </c>
       <c r="AG57" t="n">
         <v>0.0</v>
@@ -6671,7 +6671,7 @@
         <v>0.740484429065744</v>
       </c>
       <c r="K58" t="n">
-        <v>0.746726910333588</v>
+        <v>0.7467269103335877</v>
       </c>
       <c r="L58" t="n">
         <v>2.727272727272727</v>
@@ -6728,13 +6728,13 @@
         <v>-0.16315789473684197</v>
       </c>
       <c r="AD58" t="n">
-        <v>1.8888888888888888</v>
+        <v>5.0</v>
       </c>
       <c r="AE58" t="n">
-        <v>-1.0555555555555556</v>
+        <v>0.0</v>
       </c>
       <c r="AF58" t="n">
-        <v>0.6122245516114628</v>
+        <v>1.0</v>
       </c>
       <c r="AG58" t="n">
         <v>0.0</v>
@@ -6772,7 +6772,7 @@
         <v>0.7121212121212122</v>
       </c>
       <c r="K59" t="n">
-        <v>0.6864100233833473</v>
+        <v>0.6864100233833476</v>
       </c>
       <c r="L59" t="n">
         <v>2.7222222222222223</v>
@@ -6829,13 +6829,13 @@
         <v>-0.2</v>
       </c>
       <c r="AD59" t="n">
-        <v>1.8461538461538463</v>
+        <v>4.0</v>
       </c>
       <c r="AE59" t="n">
-        <v>-0.5384615384615384</v>
+        <v>0.0</v>
       </c>
       <c r="AF59" t="n">
-        <v>0.6287299445194181</v>
+        <v>1.0</v>
       </c>
       <c r="AG59" t="n">
         <v>0.0</v>
@@ -6873,7 +6873,7 @@
         <v>0.5250544662309368</v>
       </c>
       <c r="K60" t="n">
-        <v>0.6096235412027469</v>
+        <v>0.6096235412027468</v>
       </c>
       <c r="L60" t="n">
         <v>3.408333333333333</v>
@@ -6930,16 +6930,16 @@
         <v>-0.29166666666666674</v>
       </c>
       <c r="AD60" t="n">
-        <v>3.263157894736842</v>
+        <v>6.0</v>
       </c>
       <c r="AE60" t="n">
-        <v>-1.368421052631579</v>
+        <v>-3.0</v>
       </c>
       <c r="AF60" t="n">
-        <v>0.6880745776766</v>
+        <v>1.0</v>
       </c>
       <c r="AG60" t="n">
-        <v>0.40325814536340854</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="61">
@@ -6974,7 +6974,7 @@
         <v>0.4696969696969697</v>
       </c>
       <c r="K61" t="n">
-        <v>0.6303361469402874</v>
+        <v>0.6303361469402875</v>
       </c>
       <c r="L61" t="n">
         <v>2.65</v>
@@ -7031,13 +7031,13 @@
         <v>-0.13043478260869637</v>
       </c>
       <c r="AD61" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="AE61" t="n">
-        <v>-0.6923076923076923</v>
+        <v>0.0</v>
       </c>
       <c r="AF61" t="n">
-        <v>0.731449842155488</v>
+        <v>1.0</v>
       </c>
       <c r="AG61" t="n">
         <v>0.0</v>
@@ -7132,16 +7132,16 @@
         <v>-0.7763157894736843</v>
       </c>
       <c r="AD62" t="n">
-        <v>2.3076923076923075</v>
+        <v>12.0</v>
       </c>
       <c r="AE62" t="n">
-        <v>0.6923076923076923</v>
+        <v>0.0</v>
       </c>
       <c r="AF62" t="n">
-        <v>0.5698214828649613</v>
+        <v>1.0</v>
       </c>
       <c r="AG62" t="n">
-        <v>0.6757575757575759</v>
+        <v>0.0454545454545455</v>
       </c>
     </row>
     <row r="63">
@@ -7233,16 +7233,16 @@
         <v>-0.3315128345166575</v>
       </c>
       <c r="AD63" t="n">
-        <v>2.4210526315789473</v>
+        <v>10.0</v>
       </c>
       <c r="AE63" t="n">
-        <v>-0.6842105263157895</v>
+        <v>0.0</v>
       </c>
       <c r="AF63" t="n">
-        <v>0.5949563429154252</v>
+        <v>1.0</v>
       </c>
       <c r="AG63" t="n">
-        <v>0.30740740740740735</v>
+        <v>0.0222222222222222</v>
       </c>
     </row>
     <row r="64">
@@ -7334,16 +7334,16 @@
         <v>-0.3267882187938283</v>
       </c>
       <c r="AD64" t="n">
-        <v>3.142857142857143</v>
+        <v>5.0</v>
       </c>
       <c r="AE64" t="n">
-        <v>-1.0</v>
+        <v>-3.0</v>
       </c>
       <c r="AF64" t="n">
-        <v>0.7296513894066733</v>
+        <v>1.0</v>
       </c>
       <c r="AG64" t="n">
-        <v>0.4818181818181818</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="65">
@@ -7378,7 +7378,7 @@
         <v>0.6883830455259027</v>
       </c>
       <c r="K65" t="n">
-        <v>0.7670059672747954</v>
+        <v>0.7670059672747956</v>
       </c>
       <c r="L65" t="n">
         <v>4.764705882352941</v>
@@ -7435,13 +7435,13 @@
         <v>-0.9444444444444444</v>
       </c>
       <c r="AD65" t="n">
-        <v>1.8666666666666667</v>
+        <v>2.0</v>
       </c>
       <c r="AE65" t="n">
-        <v>-0.4</v>
+        <v>0.0</v>
       </c>
       <c r="AF65" t="n">
-        <v>0.6936707374093941</v>
+        <v>0.961538461538461</v>
       </c>
       <c r="AG65" t="n">
         <v>0.0</v>
@@ -7479,7 +7479,7 @@
         <v>0.6111111111111112</v>
       </c>
       <c r="K66" t="n">
-        <v>0.6518436414268679</v>
+        <v>0.6518436414268681</v>
       </c>
       <c r="L66" t="n">
         <v>3.806451612903226</v>
@@ -7536,16 +7536,16 @@
         <v>-0.6129032258064515</v>
       </c>
       <c r="AD66" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="AE66" t="n">
-        <v>-1.5384615384615385</v>
+        <v>-3.0</v>
       </c>
       <c r="AF66" t="n">
-        <v>0.660036636780582</v>
+        <v>1.0</v>
       </c>
       <c r="AG66" t="n">
-        <v>0.2666666666666668</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="67">
@@ -7580,7 +7580,7 @@
         <v>0.6301775147928994</v>
       </c>
       <c r="K67" t="n">
-        <v>0.6487310688403933</v>
+        <v>0.6487310688403936</v>
       </c>
       <c r="L67" t="n">
         <v>2.967741935483871</v>
@@ -7637,13 +7637,13 @@
         <v>-0.4313099041533548</v>
       </c>
       <c r="AD67" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="AE67" t="n">
-        <v>-1.0</v>
+        <v>-2.0</v>
       </c>
       <c r="AF67" t="n">
-        <v>0.6407596371882086</v>
+        <v>1.0</v>
       </c>
       <c r="AG67" t="n">
         <v>0.0</v>
@@ -7681,7 +7681,7 @@
         <v>0.5907297830374754</v>
       </c>
       <c r="K68" t="n">
-        <v>0.6972948089468826</v>
+        <v>0.6972948089468821</v>
       </c>
       <c r="L68" t="n">
         <v>4.645161290322581</v>
@@ -7738,16 +7738,16 @@
         <v>-0.41830065359477103</v>
       </c>
       <c r="AD68" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="AE68" t="n">
-        <v>-0.7142857142857143</v>
+        <v>0.0</v>
       </c>
       <c r="AF68" t="n">
-        <v>0.6638271460641795</v>
+        <v>1.0</v>
       </c>
       <c r="AG68" t="n">
-        <v>0.19047619047619058</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="69">
@@ -7782,7 +7782,7 @@
         <v>0.4751683501683501</v>
       </c>
       <c r="K69" t="n">
-        <v>0.6995900777392826</v>
+        <v>0.699590077739283</v>
       </c>
       <c r="L69" t="n">
         <v>1.8157894736842106</v>
@@ -7839,16 +7839,16 @@
         <v>-0.16031746031746022</v>
       </c>
       <c r="AD69" t="n">
-        <v>2.6153846153846154</v>
+        <v>6.0</v>
       </c>
       <c r="AE69" t="n">
-        <v>-1.6153846153846154</v>
+        <v>0.0</v>
       </c>
       <c r="AF69" t="n">
-        <v>0.7086869556619251</v>
+        <v>0.954545454545454</v>
       </c>
       <c r="AG69" t="n">
-        <v>0.2606060606060606</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="70">
@@ -7883,7 +7883,7 @@
         <v>1.0</v>
       </c>
       <c r="K70" t="n">
-        <v>0.7759907622602039</v>
+        <v>0.7759907622602042</v>
       </c>
       <c r="L70" t="n">
         <v>4.425531914893617</v>
@@ -7940,13 +7940,13 @@
         <v>-1.0</v>
       </c>
       <c r="AD70" t="n">
-        <v>1.8461538461538463</v>
+        <v>12.0</v>
       </c>
       <c r="AE70" t="n">
-        <v>-1.3846153846153846</v>
+        <v>-3.0</v>
       </c>
       <c r="AF70" t="n">
-        <v>0.5585284280936459</v>
+        <v>1.0</v>
       </c>
       <c r="AG70" t="n">
         <v>0.0</v>
@@ -7984,7 +7984,7 @@
         <v>0.1671085858585859</v>
       </c>
       <c r="K71" t="n">
-        <v>0.41501885289083923</v>
+        <v>0.4150188528908394</v>
       </c>
       <c r="L71" t="n">
         <v>4.8977272727272725</v>
@@ -8039,16 +8039,16 @@
         <v>-0.4635520212060964</v>
       </c>
       <c r="AD71" t="n">
-        <v>6.461538461538462</v>
+        <v>4.0</v>
       </c>
       <c r="AE71" t="n">
         <v>-3.0</v>
       </c>
       <c r="AF71" t="n">
-        <v>0.7087044534412955</v>
+        <v>0.6</v>
       </c>
       <c r="AG71" t="n">
-        <v>0.8103452103452103</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="72">
@@ -8083,7 +8083,7 @@
         <v>0.40622895622895616</v>
       </c>
       <c r="K72" t="n">
-        <v>0.589029733534097</v>
+        <v>0.5890297335340973</v>
       </c>
       <c r="L72" t="n">
         <v>6.423076923076923</v>
@@ -8140,16 +8140,16 @@
         <v>-0.3617472434266336</v>
       </c>
       <c r="AD72" t="n">
-        <v>4.0</v>
+        <v>10.0</v>
       </c>
       <c r="AE72" t="n">
-        <v>-2.769230769230769</v>
+        <v>0.0</v>
       </c>
       <c r="AF72" t="n">
-        <v>0.688754312244895</v>
+        <v>1.0</v>
       </c>
       <c r="AG72" t="n">
-        <v>0.5042735042735043</v>
+        <v>0.222222222222222</v>
       </c>
     </row>
     <row r="73">
@@ -8184,7 +8184,7 @@
         <v>0.5128205128205128</v>
       </c>
       <c r="K73" t="n">
-        <v>0.6541075676695756</v>
+        <v>0.6541075676695761</v>
       </c>
       <c r="L73" t="n">
         <v>5.931818181818182</v>
@@ -8241,16 +8241,16 @@
         <v>-0.21794871794871837</v>
       </c>
       <c r="AD73" t="n">
-        <v>2.142857142857143</v>
+        <v>4.0</v>
       </c>
       <c r="AE73" t="n">
-        <v>-1.0</v>
+        <v>-3.0</v>
       </c>
       <c r="AF73" t="n">
-        <v>0.6878842371819917</v>
+        <v>1.0</v>
       </c>
       <c r="AG73" t="n">
-        <v>0.3</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="74">
@@ -8285,7 +8285,7 @@
         <v>0.7840909090909091</v>
       </c>
       <c r="K74" t="n">
-        <v>0.7419526491669418</v>
+        <v>0.741952649166942</v>
       </c>
       <c r="L74" t="n">
         <v>3.9622641509433962</v>
@@ -8342,13 +8342,13 @@
         <v>-0.4</v>
       </c>
       <c r="AD74" t="n">
-        <v>1.8461538461538463</v>
+        <v>6.0</v>
       </c>
       <c r="AE74" t="n">
-        <v>-0.7692307692307693</v>
+        <v>0.0</v>
       </c>
       <c r="AF74" t="n">
-        <v>0.6170822281167109</v>
+        <v>1.0</v>
       </c>
       <c r="AG74" t="n">
         <v>0.0</v>
@@ -8386,7 +8386,7 @@
         <v>0.6856060606060606</v>
       </c>
       <c r="K75" t="n">
-        <v>0.6903631718354523</v>
+        <v>0.690363171835452</v>
       </c>
       <c r="L75" t="n">
         <v>1.72</v>
@@ -8443,13 +8443,13 @@
         <v>-0.07784431137724564</v>
       </c>
       <c r="AD75" t="n">
-        <v>1.8461538461538463</v>
+        <v>4.0</v>
       </c>
       <c r="AE75" t="n">
-        <v>-0.38461538461538464</v>
+        <v>-3.0</v>
       </c>
       <c r="AF75" t="n">
-        <v>0.6382940684759759</v>
+        <v>1.0</v>
       </c>
       <c r="AG75" t="n">
         <v>0.0</v>
@@ -8487,7 +8487,7 @@
         <v>0.39730639730639733</v>
       </c>
       <c r="K76" t="n">
-        <v>0.6646145954904615</v>
+        <v>0.6646145954904611</v>
       </c>
       <c r="L76" t="n">
         <v>3.475</v>
@@ -8544,16 +8544,16 @@
         <v>-0.3017319963536909</v>
       </c>
       <c r="AD76" t="n">
-        <v>3.230769230769231</v>
+        <v>2.0</v>
       </c>
       <c r="AE76" t="n">
-        <v>-0.7692307692307693</v>
+        <v>0.0</v>
       </c>
       <c r="AF76" t="n">
-        <v>0.7634822288522587</v>
+        <v>0.869565217391304</v>
       </c>
       <c r="AG76" t="n">
-        <v>0.6626984126984128</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="77">
@@ -8645,13 +8645,13 @@
         <v>-0.2</v>
       </c>
       <c r="AD77" t="n">
-        <v>1.8461538461538463</v>
+        <v>4.0</v>
       </c>
       <c r="AE77" t="n">
-        <v>-1.6153846153846154</v>
+        <v>0.0</v>
       </c>
       <c r="AF77" t="n">
-        <v>0.6287299445194181</v>
+        <v>1.0</v>
       </c>
       <c r="AG77" t="n">
         <v>0.0</v>
@@ -8689,7 +8689,7 @@
         <v>0.8421717171717171</v>
       </c>
       <c r="K78" t="n">
-        <v>0.7633270405226221</v>
+        <v>0.7633270405226223</v>
       </c>
       <c r="L78" t="n">
         <v>3.48</v>
@@ -8744,13 +8744,13 @@
         <v>-0.6560885608856084</v>
       </c>
       <c r="AD78" t="n">
-        <v>1.8461538461538463</v>
+        <v>2.0</v>
       </c>
       <c r="AE78" t="n">
         <v>-3.0</v>
       </c>
       <c r="AF78" t="n">
-        <v>0.607838827838828</v>
+        <v>0.64</v>
       </c>
       <c r="AG78" t="n">
         <v>0.0</v>
@@ -8788,7 +8788,7 @@
         <v>0.5851239669421487</v>
       </c>
       <c r="K79" t="n">
-        <v>0.6929632483024004</v>
+        <v>0.6929632483024006</v>
       </c>
       <c r="L79" t="n">
         <v>1.7272727272727273</v>
@@ -8845,13 +8845,13 @@
         <v>-0.16260162601626008</v>
       </c>
       <c r="AD79" t="n">
-        <v>1.8333333333333333</v>
+        <v>3.0</v>
       </c>
       <c r="AE79" t="n">
-        <v>-2.0</v>
+        <v>-3.0</v>
       </c>
       <c r="AF79" t="n">
-        <v>0.6816882604173121</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="AG79" t="n">
         <v>0.0</v>
@@ -8889,7 +8889,7 @@
         <v>0.7563131313131313</v>
       </c>
       <c r="K80" t="n">
-        <v>0.6818432807724646</v>
+        <v>0.6818432807724641</v>
       </c>
       <c r="L80" t="n">
         <v>1.84375</v>
@@ -8946,16 +8946,16 @@
         <v>-0.17799352750809064</v>
       </c>
       <c r="AD80" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="AE80" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="AF80" t="n">
-        <v>0.623153965461658</v>
+        <v>1.0</v>
       </c>
       <c r="AG80" t="n">
-        <v>0.33333333333333326</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="81">
@@ -8990,7 +8990,7 @@
         <v>0.42857142857142855</v>
       </c>
       <c r="K81" t="n">
-        <v>0.6470989296530397</v>
+        <v>0.6470989296530395</v>
       </c>
       <c r="L81" t="n">
         <v>2.656716417910448</v>
@@ -9047,16 +9047,16 @@
         <v>-0.3955715140634348</v>
       </c>
       <c r="AD81" t="n">
-        <v>2.933333333333333</v>
+        <v>5.0</v>
       </c>
       <c r="AE81" t="n">
-        <v>-1.1333333333333333</v>
+        <v>0.0</v>
       </c>
       <c r="AF81" t="n">
-        <v>0.6883964364475562</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="AG81" t="n">
-        <v>0.6246753246753247</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="82">
@@ -9148,13 +9148,13 @@
         <v>-1.0</v>
       </c>
       <c r="AD82" t="n">
-        <v>1.8461538461538463</v>
+        <v>12.0</v>
       </c>
       <c r="AE82" t="n">
-        <v>-2.6153846153846154</v>
+        <v>-3.0</v>
       </c>
       <c r="AF82" t="n">
-        <v>0.5585284280936459</v>
+        <v>1.0</v>
       </c>
       <c r="AG82" t="n">
         <v>0.0</v>
@@ -9192,7 +9192,7 @@
         <v>0.8907828282828283</v>
       </c>
       <c r="K83" t="n">
-        <v>0.7628503064972031</v>
+        <v>0.7628503064972033</v>
       </c>
       <c r="L83" t="n">
         <v>1.9069767441860466</v>
@@ -9249,13 +9249,13 @@
         <v>-0.582236842105263</v>
       </c>
       <c r="AD83" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="AE83" t="n">
-        <v>-1.4615384615384615</v>
+        <v>0.0</v>
       </c>
       <c r="AF83" t="n">
-        <v>0.5920233612541306</v>
+        <v>1.0</v>
       </c>
       <c r="AG83" t="n">
         <v>0.0</v>
@@ -9293,7 +9293,7 @@
         <v>0.5661718750000001</v>
       </c>
       <c r="K84" t="n">
-        <v>0.6724618248782627</v>
+        <v>0.6724618248782623</v>
       </c>
       <c r="L84" t="n">
         <v>2.6161137440758293</v>
@@ -9350,16 +9350,16 @@
         <v>-0.3609565829017203</v>
       </c>
       <c r="AD84" t="n">
-        <v>4.0</v>
+        <v>13.0</v>
       </c>
       <c r="AE84" t="n">
-        <v>-1.411764705882353</v>
+        <v>0.0</v>
       </c>
       <c r="AF84" t="n">
-        <v>0.6258907628942716</v>
+        <v>1.0</v>
       </c>
       <c r="AG84" t="n">
-        <v>0.5659622428853199</v>
+        <v>0.205128205128205</v>
       </c>
     </row>
     <row r="85">
@@ -9394,7 +9394,7 @@
         <v>0.6891679748822606</v>
       </c>
       <c r="K85" t="n">
-        <v>0.6919737827513825</v>
+        <v>0.691973782751383</v>
       </c>
       <c r="L85" t="n">
         <v>1.375</v>
@@ -9451,16 +9451,16 @@
         <v>-0.2585616438356163</v>
       </c>
       <c r="AD85" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="AE85" t="n">
-        <v>-0.4</v>
+        <v>-2.0</v>
       </c>
       <c r="AF85" t="n">
-        <v>0.6426629795416982</v>
+        <v>1.0</v>
       </c>
       <c r="AG85" t="n">
-        <v>0.2047619047619047</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="86">
@@ -9495,7 +9495,7 @@
         <v>0.6439842209072978</v>
       </c>
       <c r="K86" t="n">
-        <v>0.6286140034427037</v>
+        <v>0.6286140034427038</v>
       </c>
       <c r="L86" t="n">
         <v>3.0714285714285716</v>
@@ -9552,16 +9552,16 @@
         <v>-0.20491803278688497</v>
       </c>
       <c r="AD86" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="AE86" t="n">
-        <v>-0.7142857142857143</v>
+        <v>0.0</v>
       </c>
       <c r="AF86" t="n">
-        <v>0.6584126572703488</v>
+        <v>1.0</v>
       </c>
       <c r="AG86" t="n">
-        <v>0.1875</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="87">
@@ -9596,7 +9596,7 @@
         <v>0.18550084175084178</v>
       </c>
       <c r="K87" t="n">
-        <v>0.4892434027867939</v>
+        <v>0.4892434027867937</v>
       </c>
       <c r="L87" t="n">
         <v>7.4</v>
@@ -9653,16 +9653,16 @@
         <v>-0.0037174721189577836</v>
       </c>
       <c r="AD87" t="n">
-        <v>2.769230769230769</v>
+        <v>3.0</v>
       </c>
       <c r="AE87" t="n">
-        <v>-2.769230769230769</v>
+        <v>-3.0</v>
       </c>
       <c r="AF87" t="n">
-        <v>0.8212040908825984</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="AG87" t="n">
-        <v>0.10256410256410262</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="88">
@@ -9697,7 +9697,7 @@
         <v>0.4403453689167976</v>
       </c>
       <c r="K88" t="n">
-        <v>0.6463453681635187</v>
+        <v>0.6463453681635188</v>
       </c>
       <c r="L88" t="n">
         <v>5.966101694915254</v>
@@ -9752,16 +9752,16 @@
         <v>-0.1282798833819244</v>
       </c>
       <c r="AD88" t="n">
-        <v>2.4</v>
+        <v>5.0</v>
       </c>
       <c r="AE88" t="n">
-        <v>-2.8</v>
+        <v>-3.0</v>
       </c>
       <c r="AF88" t="n">
-        <v>0.7004205126098291</v>
+        <v>1.0</v>
       </c>
       <c r="AG88" t="n">
-        <v>0.2466666666666667</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="89">
@@ -9796,7 +9796,7 @@
         <v>0.7060439560439561</v>
       </c>
       <c r="K89" t="n">
-        <v>0.6669611518351825</v>
+        <v>0.6669611518351822</v>
       </c>
       <c r="L89" t="n">
         <v>2.127659574468085</v>
@@ -9851,16 +9851,16 @@
         <v>-0.17782909930715926</v>
       </c>
       <c r="AD89" t="n">
-        <v>2.2666666666666666</v>
+        <v>5.0</v>
       </c>
       <c r="AE89" t="n">
-        <v>-2.6</v>
+        <v>-3.0</v>
       </c>
       <c r="AF89" t="n">
-        <v>0.6357245797383172</v>
+        <v>1.0</v>
       </c>
       <c r="AG89" t="n">
-        <v>0.2727272727272727</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="90">
@@ -9952,16 +9952,16 @@
         <v>-0.5216434336023477</v>
       </c>
       <c r="AD90" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="AE90" t="n">
-        <v>-0.23529411764705882</v>
+        <v>0.0</v>
       </c>
       <c r="AF90" t="n">
-        <v>0.5842156298977327</v>
+        <v>1.0</v>
       </c>
       <c r="AG90" t="n">
-        <v>0.38888888888888884</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="91">
@@ -9996,7 +9996,7 @@
         <v>0.2819834710743802</v>
       </c>
       <c r="K91" t="n">
-        <v>0.3286017616669822</v>
+        <v>0.328601761666982</v>
       </c>
       <c r="L91" t="n">
         <v>3.2222222222222223</v>
@@ -10053,16 +10053,16 @@
         <v>-0.24271844660194175</v>
       </c>
       <c r="AD91" t="n">
-        <v>2.6666666666666665</v>
+        <v>3.0</v>
       </c>
       <c r="AE91" t="n">
-        <v>-2.25</v>
+        <v>0.0</v>
       </c>
       <c r="AF91" t="n">
-        <v>0.8135841923880718</v>
+        <v>0.84</v>
       </c>
       <c r="AG91" t="n">
-        <v>0.08333333333333325</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="92">
@@ -10097,7 +10097,7 @@
         <v>0.4972643097643097</v>
       </c>
       <c r="K92" t="n">
-        <v>0.6061860976384703</v>
+        <v>0.6061860976384705</v>
       </c>
       <c r="L92" t="n">
         <v>6.856060606060606</v>
@@ -10154,16 +10154,16 @@
         <v>-0.4539205155746513</v>
       </c>
       <c r="AD92" t="n">
-        <v>3.6923076923076925</v>
+        <v>10.0</v>
       </c>
       <c r="AE92" t="n">
-        <v>-1.1538461538461537</v>
+        <v>0.0</v>
       </c>
       <c r="AF92" t="n">
-        <v>0.6798167676886212</v>
+        <v>1.0</v>
       </c>
       <c r="AG92" t="n">
-        <v>0.6521367521367522</v>
+        <v>0.177777777777778</v>
       </c>
     </row>
     <row r="93">
@@ -10198,7 +10198,7 @@
         <v>0.5464856902356902</v>
       </c>
       <c r="K93" t="n">
-        <v>0.6728497817027043</v>
+        <v>0.6728497817027038</v>
       </c>
       <c r="L93" t="n">
         <v>4.3076923076923075</v>
@@ -10255,13 +10255,13 @@
         <v>-0.3846153846153847</v>
       </c>
       <c r="AD93" t="n">
-        <v>2.3076923076923075</v>
+        <v>6.0</v>
       </c>
       <c r="AE93" t="n">
-        <v>-2.076923076923077</v>
+        <v>-3.0</v>
       </c>
       <c r="AF93" t="n">
-        <v>0.6923347564504964</v>
+        <v>1.0</v>
       </c>
       <c r="AG93" t="n">
         <v>0.0</v>
@@ -10299,7 +10299,7 @@
         <v>0.5355371900826447</v>
       </c>
       <c r="K94" t="n">
-        <v>0.6794615015976847</v>
+        <v>0.6794615015976844</v>
       </c>
       <c r="L94" t="n">
         <v>3.696969696969697</v>
@@ -10356,13 +10356,13 @@
         <v>-0.07317073170731705</v>
       </c>
       <c r="AD94" t="n">
-        <v>1.8333333333333333</v>
+        <v>3.0</v>
       </c>
       <c r="AE94" t="n">
-        <v>-0.16666666666666666</v>
+        <v>0.0</v>
       </c>
       <c r="AF94" t="n">
-        <v>0.7010488555325511</v>
+        <v>1.0</v>
       </c>
       <c r="AG94" t="n">
         <v>0.0</v>
@@ -10400,7 +10400,7 @@
         <v>0.6382575757575758</v>
       </c>
       <c r="K95" t="n">
-        <v>0.7514790618967375</v>
+        <v>0.7514790618967372</v>
       </c>
       <c r="L95" t="n">
         <v>2.227272727272727</v>
@@ -10457,16 +10457,16 @@
         <v>-0.6833667334669334</v>
       </c>
       <c r="AD95" t="n">
-        <v>2.1538461538461537</v>
+        <v>3.0</v>
       </c>
       <c r="AE95" t="n">
-        <v>-0.5384615384615384</v>
+        <v>0.0</v>
       </c>
       <c r="AF95" t="n">
-        <v>0.6761213402460087</v>
+        <v>0.904761904761905</v>
       </c>
       <c r="AG95" t="n">
-        <v>0.41428571428571426</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="96">
@@ -10501,7 +10501,7 @@
         <v>0.8358585858585859</v>
       </c>
       <c r="K96" t="n">
-        <v>0.7243148930851242</v>
+        <v>0.7243148930851244</v>
       </c>
       <c r="L96" t="n">
         <v>2.27027027027027</v>
@@ -10558,16 +10558,16 @@
         <v>-0.5475797579757974</v>
       </c>
       <c r="AD96" t="n">
-        <v>2.6153846153846154</v>
+        <v>10.0</v>
       </c>
       <c r="AE96" t="n">
-        <v>-0.46153846153846156</v>
+        <v>0.0</v>
       </c>
       <c r="AF96" t="n">
-        <v>0.600380904742756</v>
+        <v>1.0</v>
       </c>
       <c r="AG96" t="n">
-        <v>0.7320987654320987</v>
+        <v>0.0888888888888889</v>
       </c>
     </row>
     <row r="97">
@@ -10602,7 +10602,7 @@
         <v>0.7291666666666666</v>
       </c>
       <c r="K97" t="n">
-        <v>0.7281974999558517</v>
+        <v>0.7281974999558518</v>
       </c>
       <c r="L97" t="n">
         <v>2.5238095238095237</v>
@@ -10659,16 +10659,16 @@
         <v>-0.18954248366013055</v>
       </c>
       <c r="AD97" t="n">
-        <v>2.1538461538461537</v>
+        <v>6.0</v>
       </c>
       <c r="AE97" t="n">
-        <v>-0.6153846153846154</v>
+        <v>0.0</v>
       </c>
       <c r="AF97" t="n">
-        <v>0.6256680161943321</v>
+        <v>1.0</v>
       </c>
       <c r="AG97" t="n">
-        <v>0.3523809523809523</v>
+        <v>0.133333333333333</v>
       </c>
     </row>
     <row r="98">
@@ -10703,7 +10703,7 @@
         <v>1.0</v>
       </c>
       <c r="K98" t="n">
-        <v>0.7759907622602042</v>
+        <v>0.7759907622602039</v>
       </c>
       <c r="L98" t="n">
         <v>1.0</v>
@@ -10760,13 +10760,13 @@
         <v>-1.0</v>
       </c>
       <c r="AD98" t="n">
-        <v>1.8461538461538463</v>
+        <v>12.0</v>
       </c>
       <c r="AE98" t="n">
-        <v>-0.6153846153846154</v>
+        <v>0.0</v>
       </c>
       <c r="AF98" t="n">
-        <v>0.5585284280936459</v>
+        <v>1.0</v>
       </c>
       <c r="AG98" t="n">
         <v>0.0</v>
@@ -10804,7 +10804,7 @@
         <v>0.9848484848484849</v>
       </c>
       <c r="K99" t="n">
-        <v>0.7659569903204871</v>
+        <v>0.7659569903204869</v>
       </c>
       <c r="L99" t="n">
         <v>2.4489795918367347</v>
@@ -10861,16 +10861,16 @@
         <v>-0.8935950413223142</v>
       </c>
       <c r="AD99" t="n">
-        <v>2.0</v>
+        <v>12.0</v>
       </c>
       <c r="AE99" t="n">
-        <v>-0.38461538461538464</v>
+        <v>0.0</v>
       </c>
       <c r="AF99" t="n">
-        <v>0.5621769534813016</v>
+        <v>1.0</v>
       </c>
       <c r="AG99" t="n">
-        <v>0.6717171717171717</v>
+        <v>0.0151515151515152</v>
       </c>
     </row>
     <row r="100">
@@ -10905,7 +10905,7 @@
         <v>0.9305785123966942</v>
       </c>
       <c r="K100" t="n">
-        <v>0.7717188152054522</v>
+        <v>0.7717188152054519</v>
       </c>
       <c r="L100" t="n">
         <v>1.9565217391304348</v>
@@ -10962,13 +10962,13 @@
         <v>-0.7262313860252004</v>
       </c>
       <c r="AD100" t="n">
-        <v>1.8333333333333333</v>
+        <v>9.0</v>
       </c>
       <c r="AE100" t="n">
-        <v>-1.1666666666666667</v>
+        <v>0.0</v>
       </c>
       <c r="AF100" t="n">
-        <v>0.5861105545537524</v>
+        <v>1.0</v>
       </c>
       <c r="AG100" t="n">
         <v>0.0</v>
@@ -11006,7 +11006,7 @@
         <v>0.5019723865877712</v>
       </c>
       <c r="K101" t="n">
-        <v>0.696491429139916</v>
+        <v>0.696491429139917</v>
       </c>
       <c r="L101" t="n">
         <v>1.5</v>
@@ -11063,13 +11063,13 @@
         <v>-0.15923566878980935</v>
       </c>
       <c r="AD101" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="AE101" t="n">
-        <v>-0.07142857142857142</v>
+        <v>0.0</v>
       </c>
       <c r="AF101" t="n">
-        <v>0.7064504120268517</v>
+        <v>0.88235294117647</v>
       </c>
       <c r="AG101" t="n">
         <v>0.0</v>
@@ -11107,7 +11107,7 @@
         <v>0.7563131313131313</v>
       </c>
       <c r="K102" t="n">
-        <v>0.7391624752530124</v>
+        <v>0.7391624752530125</v>
       </c>
       <c r="L102" t="n">
         <v>2.5555555555555554</v>
@@ -11164,13 +11164,13 @@
         <v>-0.08333333333333326</v>
       </c>
       <c r="AD102" t="n">
-        <v>1.8461538461538463</v>
+        <v>5.0</v>
       </c>
       <c r="AE102" t="n">
-        <v>-0.8461538461538461</v>
+        <v>0.0</v>
       </c>
       <c r="AF102" t="n">
-        <v>0.6218589267784156</v>
+        <v>1.0</v>
       </c>
       <c r="AG102" t="n">
         <v>0.0</v>
@@ -11208,7 +11208,7 @@
         <v>0.23758417508417512</v>
       </c>
       <c r="K103" t="n">
-        <v>0.5248565426737827</v>
+        <v>0.5248565426737829</v>
       </c>
       <c r="L103" t="n">
         <v>5.855555555555555</v>
@@ -11265,16 +11265,16 @@
         <v>-0.038961038961039286</v>
       </c>
       <c r="AD103" t="n">
-        <v>3.076923076923077</v>
+        <v>3.0</v>
       </c>
       <c r="AE103" t="n">
-        <v>-2.6923076923076925</v>
+        <v>0.0</v>
       </c>
       <c r="AF103" t="n">
-        <v>0.7567366449211196</v>
+        <v>0.869565217391304</v>
       </c>
       <c r="AG103" t="n">
-        <v>0.35277777777777775</v>
+        <v>0.666666666666667</v>
       </c>
     </row>
     <row r="104">
@@ -11309,7 +11309,7 @@
         <v>0.5140495867768595</v>
       </c>
       <c r="K104" t="n">
-        <v>0.503542915995974</v>
+        <v>0.5035429159959741</v>
       </c>
       <c r="L104" t="n">
         <v>4.011627906976744</v>
@@ -11366,16 +11366,16 @@
         <v>-0.12</v>
       </c>
       <c r="AD104" t="n">
-        <v>2.6666666666666665</v>
+        <v>4.0</v>
       </c>
       <c r="AE104" t="n">
-        <v>0.5</v>
+        <v>0.0</v>
       </c>
       <c r="AF104" t="n">
-        <v>0.7038043192231723</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="AG104" t="n">
-        <v>0.2266666666666666</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="105">
@@ -11410,7 +11410,7 @@
         <v>0.5088383838383839</v>
       </c>
       <c r="K105" t="n">
-        <v>0.5298498999513519</v>
+        <v>0.5298498999513523</v>
       </c>
       <c r="L105" t="n">
         <v>2.2045454545454546</v>
@@ -11467,16 +11467,16 @@
         <v>-0.26378896882493935</v>
       </c>
       <c r="AD105" t="n">
-        <v>2.6153846153846154</v>
+        <v>4.0</v>
       </c>
       <c r="AE105" t="n">
         <v>-1.0</v>
       </c>
       <c r="AF105" t="n">
-        <v>0.7168803672576528</v>
+        <v>1.0</v>
       </c>
       <c r="AG105" t="n">
-        <v>0.5222222222222223</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="106">
@@ -11568,13 +11568,13 @@
         <v>-0.6754966887417219</v>
       </c>
       <c r="AD106" t="n">
-        <v>1.8333333333333333</v>
+        <v>3.0</v>
       </c>
       <c r="AE106" t="n">
-        <v>-1.5</v>
+        <v>0.0</v>
       </c>
       <c r="AF106" t="n">
-        <v>0.6745602093045053</v>
+        <v>1.0</v>
       </c>
       <c r="AG106" t="n">
         <v>0.0</v>
@@ -11612,7 +11612,7 @@
         <v>0.577020202020202</v>
       </c>
       <c r="K107" t="n">
-        <v>0.5919173910257378</v>
+        <v>0.5919173910257381</v>
       </c>
       <c r="L107" t="n">
         <v>2.7625</v>
@@ -11669,16 +11669,16 @@
         <v>-0.20491803278688578</v>
       </c>
       <c r="AD107" t="n">
-        <v>3.230769230769231</v>
+        <v>7.0</v>
       </c>
       <c r="AE107" t="n">
-        <v>-1.4615384615384615</v>
+        <v>0.0</v>
       </c>
       <c r="AF107" t="n">
-        <v>0.6800009236017288</v>
+        <v>1.0</v>
       </c>
       <c r="AG107" t="n">
-        <v>0.3827838827838827</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="108">
@@ -11713,7 +11713,7 @@
         <v>0.509469696969697</v>
       </c>
       <c r="K108" t="n">
-        <v>0.6856155533238778</v>
+        <v>0.6856155533238777</v>
       </c>
       <c r="L108" t="n">
         <v>2.8</v>
@@ -11770,16 +11770,16 @@
         <v>-0.2414089347079042</v>
       </c>
       <c r="AD108" t="n">
-        <v>2.6153846153846154</v>
+        <v>7.0</v>
       </c>
       <c r="AE108" t="n">
-        <v>-1.3076923076923077</v>
+        <v>0.0</v>
       </c>
       <c r="AF108" t="n">
-        <v>0.6607293401467531</v>
+        <v>1.0</v>
       </c>
       <c r="AG108" t="n">
-        <v>0.5130952380952379</v>
+        <v>0.238095238095238</v>
       </c>
     </row>
     <row r="109">
@@ -11814,7 +11814,7 @@
         <v>1.0</v>
       </c>
       <c r="K109" t="n">
-        <v>0.775990762260204</v>
+        <v>0.7759907622602042</v>
       </c>
       <c r="L109" t="n">
         <v>1.6923076923076923</v>
@@ -11871,13 +11871,13 @@
         <v>-1.0</v>
       </c>
       <c r="AD109" t="n">
-        <v>1.8461538461538463</v>
+        <v>12.0</v>
       </c>
       <c r="AE109" t="n">
-        <v>-1.3076923076923077</v>
+        <v>0.0</v>
       </c>
       <c r="AF109" t="n">
-        <v>0.5585284280936459</v>
+        <v>1.0</v>
       </c>
       <c r="AG109" t="n">
         <v>0.0</v>
@@ -11972,13 +11972,13 @@
         <v>-0.26829268292682923</v>
       </c>
       <c r="AD110" t="n">
-        <v>2.1538461538461537</v>
+        <v>6.0</v>
       </c>
       <c r="AE110" t="n">
-        <v>-1.1538461538461537</v>
+        <v>-1.0</v>
       </c>
       <c r="AF110" t="n">
-        <v>0.645797906405847</v>
+        <v>1.0</v>
       </c>
       <c r="AG110" t="n">
         <v>0.0</v>
@@ -12073,16 +12073,16 @@
         <v>-0.30789049919484696</v>
       </c>
       <c r="AD111" t="n">
-        <v>4.769230769230769</v>
+        <v>12.0</v>
       </c>
       <c r="AE111" t="n">
-        <v>-0.07692307692307693</v>
+        <v>0.0</v>
       </c>
       <c r="AF111" t="n">
-        <v>0.636791278896542</v>
+        <v>1.0</v>
       </c>
       <c r="AG111" t="n">
-        <v>0.7965034965034965</v>
+        <v>0.287878787878788</v>
       </c>
     </row>
     <row r="112">
@@ -12117,7 +12117,7 @@
         <v>0.8533333333333334</v>
       </c>
       <c r="K112" t="n">
-        <v>0.7896680211760521</v>
+        <v>0.7896680211760522</v>
       </c>
       <c r="L112" t="n">
         <v>1.3181818181818181</v>
@@ -12174,13 +12174,13 @@
         <v>-0.3530066815144768</v>
       </c>
       <c r="AD112" t="n">
-        <v>1.875</v>
+        <v>8.0</v>
       </c>
       <c r="AE112" t="n">
-        <v>-1.375</v>
+        <v>-2.0</v>
       </c>
       <c r="AF112" t="n">
-        <v>0.5898470801364023</v>
+        <v>1.0</v>
       </c>
       <c r="AG112" t="n">
         <v>0.0</v>
@@ -12275,13 +12275,13 @@
         <v>-0.43181818181818177</v>
       </c>
       <c r="AD113" t="n">
-        <v>1.8333333333333333</v>
+        <v>6.0</v>
       </c>
       <c r="AE113" t="n">
-        <v>-1.75</v>
+        <v>0.0</v>
       </c>
       <c r="AF113" t="n">
-        <v>0.6198295168883403</v>
+        <v>1.0</v>
       </c>
       <c r="AG113" t="n">
         <v>0.0</v>
@@ -12319,7 +12319,7 @@
         <v>0.5252525252525253</v>
       </c>
       <c r="K114" t="n">
-        <v>0.6922340897759259</v>
+        <v>0.6922340897759256</v>
       </c>
       <c r="L114" t="n">
         <v>1.8571428571428572</v>
@@ -12376,13 +12376,13 @@
         <v>0.07874015748031477</v>
       </c>
       <c r="AD114" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="AE114" t="n">
-        <v>0.15384615384615385</v>
+        <v>0.0</v>
       </c>
       <c r="AF114" t="n">
-        <v>0.6861820920710676</v>
+        <v>1.0</v>
       </c>
       <c r="AG114" t="n">
         <v>0.0</v>
@@ -12420,7 +12420,7 @@
         <v>0.6760330578512397</v>
       </c>
       <c r="K115" t="n">
-        <v>0.6817290787845062</v>
+        <v>0.6817290787845063</v>
       </c>
       <c r="L115" t="n">
         <v>3.4516129032258065</v>
@@ -12477,16 +12477,16 @@
         <v>-0.10638297872340459</v>
       </c>
       <c r="AD115" t="n">
-        <v>2.1666666666666665</v>
+        <v>5.0</v>
       </c>
       <c r="AE115" t="n">
-        <v>-1.0833333333333333</v>
+        <v>0.0</v>
       </c>
       <c r="AF115" t="n">
-        <v>0.6543145212630506</v>
+        <v>1.0</v>
       </c>
       <c r="AG115" t="n">
-        <v>0.3476190476190477</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="116">
@@ -12521,7 +12521,7 @@
         <v>0.7171717171717171</v>
       </c>
       <c r="K116" t="n">
-        <v>0.7161395173470759</v>
+        <v>0.7161395173470756</v>
       </c>
       <c r="L116" t="n">
         <v>6.3076923076923075</v>
@@ -12578,16 +12578,16 @@
         <v>-0.44302325581395346</v>
       </c>
       <c r="AD116" t="n">
-        <v>2.6153846153846154</v>
+        <v>9.0</v>
       </c>
       <c r="AE116" t="n">
-        <v>-0.46153846153846156</v>
+        <v>0.0</v>
       </c>
       <c r="AF116" t="n">
-        <v>0.627963830656715</v>
+        <v>1.0</v>
       </c>
       <c r="AG116" t="n">
-        <v>0.275</v>
+        <v>0.0833333333333333</v>
       </c>
     </row>
     <row r="117">
@@ -12622,7 +12622,7 @@
         <v>0.5997474747474747</v>
       </c>
       <c r="K117" t="n">
-        <v>0.6402035492877842</v>
+        <v>0.640203549287784</v>
       </c>
       <c r="L117" t="n">
         <v>4.785714285714286</v>
@@ -12679,13 +12679,13 @@
         <v>-0.7528089887640448</v>
       </c>
       <c r="AD117" t="n">
-        <v>1.8461538461538463</v>
+        <v>3.0</v>
       </c>
       <c r="AE117" t="n">
-        <v>1.3076923076923077</v>
+        <v>0.0</v>
       </c>
       <c r="AF117" t="n">
-        <v>0.6624860067167762</v>
+        <v>1.0</v>
       </c>
       <c r="AG117" t="n">
         <v>0.0</v>
@@ -12780,16 +12780,16 @@
         <v>-0.5413402959094862</v>
       </c>
       <c r="AD118" t="n">
-        <v>2.8</v>
+        <v>6.0</v>
       </c>
       <c r="AE118" t="n">
-        <v>-0.4666666666666667</v>
+        <v>-3.0</v>
       </c>
       <c r="AF118" t="n">
-        <v>0.653583103534084</v>
+        <v>0.863636363636364</v>
       </c>
       <c r="AG118" t="n">
-        <v>0.5318181818181819</v>
+        <v>0.266666666666667</v>
       </c>
     </row>
     <row r="119">
@@ -12824,7 +12824,7 @@
         <v>0.5147174254317112</v>
       </c>
       <c r="K119" t="n">
-        <v>0.5581881001638296</v>
+        <v>0.5581881001638294</v>
       </c>
       <c r="L119" t="n">
         <v>3.323943661971831</v>
@@ -12881,16 +12881,16 @@
         <v>0.0011098779134287855</v>
       </c>
       <c r="AD119" t="n">
-        <v>3.3333333333333335</v>
+        <v>6.0</v>
       </c>
       <c r="AE119" t="n">
-        <v>-0.26666666666666666</v>
+        <v>0.0</v>
       </c>
       <c r="AF119" t="n">
-        <v>0.6846499322527755</v>
+        <v>1.0</v>
       </c>
       <c r="AG119" t="n">
-        <v>0.49555555555555547</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="120">
@@ -12925,7 +12925,7 @@
         <v>0.5611439842209073</v>
       </c>
       <c r="K120" t="n">
-        <v>0.6462097425793838</v>
+        <v>0.6462097425793841</v>
       </c>
       <c r="L120" t="n">
         <v>2.5</v>
@@ -12982,16 +12982,16 @@
         <v>-0.6054054054054059</v>
       </c>
       <c r="AD120" t="n">
-        <v>2.5714285714285716</v>
+        <v>2.0</v>
       </c>
       <c r="AE120" t="n">
-        <v>-1.5</v>
+        <v>-3.0</v>
       </c>
       <c r="AF120" t="n">
-        <v>0.6972466975425242</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="AG120" t="n">
-        <v>0.4222222222222222</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="121">
@@ -13026,7 +13026,7 @@
         <v>0.32386363636363635</v>
       </c>
       <c r="K121" t="n">
-        <v>0.5757134300352925</v>
+        <v>0.5757134300352917</v>
       </c>
       <c r="L121" t="n">
         <v>6.988095238095238</v>
@@ -13083,16 +13083,16 @@
         <v>-0.05865522174535</v>
       </c>
       <c r="AD121" t="n">
-        <v>3.076923076923077</v>
+        <v>6.0</v>
       </c>
       <c r="AE121" t="n">
-        <v>-0.3076923076923077</v>
+        <v>-2.0</v>
       </c>
       <c r="AF121" t="n">
-        <v>0.7237985064948507</v>
+        <v>1.0</v>
       </c>
       <c r="AG121" t="n">
-        <v>0.20277777777777767</v>
+        <v>0.133333333333333</v>
       </c>
     </row>
     <row r="122">
@@ -13127,7 +13127,7 @@
         <v>0.4810606060606061</v>
       </c>
       <c r="K122" t="n">
-        <v>0.640015748728792</v>
+        <v>0.6400157487287917</v>
       </c>
       <c r="L122" t="n">
         <v>1.3888888888888888</v>
@@ -13184,13 +13184,13 @@
         <v>0.18644067796610206</v>
       </c>
       <c r="AD122" t="n">
-        <v>1.8461538461538463</v>
+        <v>3.0</v>
       </c>
       <c r="AE122" t="n">
-        <v>-1.4615384615384615</v>
+        <v>0.0</v>
       </c>
       <c r="AF122" t="n">
-        <v>0.7031294534886344</v>
+        <v>0.90625</v>
       </c>
       <c r="AG122" t="n">
         <v>0.0</v>

</xml_diff>